<commit_message>
Added tags in alphabetical order
</commit_message>
<xml_diff>
--- a/HTML5_Tags.xlsx
+++ b/HTML5_Tags.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\users.cpcc.edu\users\MAC9812E\CPCC\WEB215\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Desktop\CPCC\WEB215\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFB9725-0D92-4B40-A4B9-296028EB457D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="444">
   <si>
     <t>Tag</t>
   </si>
@@ -672,12 +673,696 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Paragraph</t>
+  </si>
+  <si>
+    <t>Form/Table</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Code/Ruby</t>
+  </si>
+  <si>
+    <t>HTML Format</t>
+  </si>
+  <si>
+    <t>&amp;lt;!--...--&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;!DOCTYPE&gt;&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;a&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;abbr&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;address&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;area&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;article&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;aside&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;audio&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;b&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;base&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;bdi&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;bdo&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;blockquote&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;body&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;br&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;button&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;canvas&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;caption&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;cite&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;code&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;col&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;colgroup&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;data&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;datalist&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;dd&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;del&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;details&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;dfn&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;dialog&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;div&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;dl&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;dt&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;em&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;embed&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;fieldset&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;figcaption&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;figure&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;footer&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;form&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;h1&gt; to &lt;h6&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;head&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;header&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;hr&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;html&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;i&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;iframe&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;img&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;input&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;ins&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;kbd&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;label&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;legend&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;li&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;link&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;main&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;map&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;mark&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;meta&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;meter&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;nav&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;noscript&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;object&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;ol&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;optgroup&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;option&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;output&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;p&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;param&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;picture&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;pre&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;progress&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;q&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;rp&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;rt&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;ruby&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;s&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;samp&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;script&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;section&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;select&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;small&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;source&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;span&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;strong&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;style&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;sub&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;summary&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;sup&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;svg&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;table&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;tbody&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;td&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;template&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;textarea&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;tfoot&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;th&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;thead&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;time&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;title&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;tr&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;track&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;u&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;ul&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;var&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;video&amp;gt;</t>
+  </si>
+  <si>
+    <t>&amp;lt;wbr&amp;gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;!--...--&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;!DOCTYPE&gt;&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;a&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;abbr&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;address&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;area&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;article&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;aside&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;audio&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;b&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;base&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;bdi&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;bdo&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;blockquote&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;body&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;br&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;button&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;canvas&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;caption&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;cite&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;code&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;col&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;colgroup&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;data&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;datalist&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;dd&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;del&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;details&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;dfn&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;dialog&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;div&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;dl&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;dt&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;em&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;embed&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;fieldset&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;figcaption&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;figure&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;footer&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;form&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;h1&gt; to &lt;h6&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;head&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;header&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;hr&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;html&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;i&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;iframe&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;img&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;input&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;ins&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;kbd&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;label&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;legend&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;li&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;link&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;main&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;map&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;mark&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;meta&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;meter&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;nav&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;noscript&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;object&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;ol&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;optgroup&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;option&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;output&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;p&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;param&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;picture&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;pre&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;progress&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;q&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;rp&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;rt&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;ruby&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;s&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;samp&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;script&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;section&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;select&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;small&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;source&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;span&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;strong&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;style&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;sub&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;summary&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;sup&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;svg&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;table&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;tbody&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;td&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;template&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;textarea&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;tfoot&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;th&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;thead&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;time&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;title&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;tr&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;track&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;u&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;ul&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;var&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;video&amp;gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;&amp;lt;wbr&amp;gt;&lt;/li&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -791,7 +1476,94 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFDDDDDD"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -893,19 +1665,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C108" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:C108">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A2:C108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F108" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:F108" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:F108">
     <sortCondition ref="B1:B108"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Used"/>
-    <tableColumn id="2" name="Tag" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Used"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tag" dataDxfId="4" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{10EDB6FF-0161-4643-B1E0-D5D22A6DAB01}" name="Category" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{67C496C7-E207-4AEC-8F74-F9F814F59A6A}" name="HTML Format" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00E6A6D7-58A3-459A-AC1D-2DB8EFF77B7E}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1173,20 +1944,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="117.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="117.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>214</v>
       </c>
@@ -1194,18 +1968,36 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -1213,10 +2005,19 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -1224,34 +2025,68 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -1259,29 +2094,56 @@
         <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>215</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -1289,10 +2151,19 @@
         <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -1300,34 +2171,70 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -1335,53 +2242,107 @@
         <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>215</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -1389,82 +2350,160 @@
         <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -1472,26 +2511,53 @@
         <v>62</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -1499,53 +2565,103 @@
         <v>68</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>215</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>215</v>
       </c>
@@ -1553,10 +2669,19 @@
         <v>80</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>215</v>
       </c>
@@ -1564,10 +2689,19 @@
         <v>82</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -1575,40 +2709,74 @@
         <v>84</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>215</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>215</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>215</v>
       </c>
@@ -1616,18 +2784,34 @@
         <v>92</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>215</v>
       </c>
@@ -1635,10 +2819,19 @@
         <v>96</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>215</v>
       </c>
@@ -1646,26 +2839,49 @@
         <v>98</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>215</v>
       </c>
@@ -1673,18 +2889,34 @@
         <v>104</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>215</v>
       </c>
@@ -1692,21 +2924,37 @@
         <v>108</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>215</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>215</v>
       </c>
@@ -1714,45 +2962,84 @@
         <v>112</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C59" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>215</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="F61" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -1760,26 +3047,51 @@
         <v>122</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -1787,61 +3099,118 @@
         <v>128</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>215</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="F71" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -1849,66 +3218,132 @@
         <v>142</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="4"/>
+      <c r="D73" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>146</v>
       </c>
       <c r="C74" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C75" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C77" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F77" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="4"/>
+      <c r="D78" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="4"/>
+      <c r="D79" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="F79" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>215</v>
       </c>
@@ -1916,10 +3351,19 @@
         <v>158</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F80" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>215</v>
       </c>
@@ -1927,42 +3371,87 @@
         <v>160</v>
       </c>
       <c r="C81" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F81" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C82" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C83" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="F83" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C84" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>215</v>
       </c>
@@ -1970,122 +3459,253 @@
         <v>168</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C87" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C88" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="F88" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C89" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="F89" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C90" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="F90" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F91" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F92" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="4"/>
+      <c r="D95" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="F95" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C96" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="F97" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C98" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F98" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C99" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="F99" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="4"/>
+      <c r="D100" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="F100" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>215</v>
       </c>
@@ -2093,34 +3713,70 @@
         <v>198</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F101" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C102" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="F102" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C103" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F103" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C104" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="F104" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>215</v>
       </c>
@@ -2128,142 +3784,174 @@
         <v>206</v>
       </c>
       <c r="C105" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="F105" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="4"/>
+      <c r="D106" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F106" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F107" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="4"/>
+      <c r="D108" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.w3schools.com/tags/tag_comment.asp"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.w3schools.com/tags/tag_doctype.asp"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.w3schools.com/tags/tag_a.asp"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www.w3schools.com/tags/tag_abbr.asp"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://www.w3schools.com/tags/tag_address.asp"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.w3schools.com/tags/tag_area.asp"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://www.w3schools.com/tags/tag_article.asp"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.w3schools.com/tags/tag_aside.asp"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.w3schools.com/tags/tag_audio.asp"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.w3schools.com/tags/tag_b.asp"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://www.w3schools.com/tags/tag_base.asp"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://www.w3schools.com/tags/tag_bdi.asp"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://www.w3schools.com/tags/tag_bdo.asp"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://www.w3schools.com/tags/tag_blockquote.asp"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://www.w3schools.com/tags/tag_body.asp"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://www.w3schools.com/tags/tag_br.asp"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://www.w3schools.com/tags/tag_button.asp"/>
-    <hyperlink ref="B19" r:id="rId18" display="https://www.w3schools.com/tags/tag_canvas.asp"/>
-    <hyperlink ref="B20" r:id="rId19" display="https://www.w3schools.com/tags/tag_caption.asp"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://www.w3schools.com/tags/tag_cite.asp"/>
-    <hyperlink ref="B22" r:id="rId21" display="https://www.w3schools.com/tags/tag_code.asp"/>
-    <hyperlink ref="B23" r:id="rId22" display="https://www.w3schools.com/tags/tag_col.asp"/>
-    <hyperlink ref="B24" r:id="rId23" display="https://www.w3schools.com/tags/tag_colgroup.asp"/>
-    <hyperlink ref="B25" r:id="rId24" display="https://www.w3schools.com/tags/tag_data.asp"/>
-    <hyperlink ref="B26" r:id="rId25" display="https://www.w3schools.com/tags/tag_datalist.asp"/>
-    <hyperlink ref="B27" r:id="rId26" display="https://www.w3schools.com/tags/tag_dd.asp"/>
-    <hyperlink ref="B28" r:id="rId27" display="https://www.w3schools.com/tags/tag_del.asp"/>
-    <hyperlink ref="B29" r:id="rId28" display="https://www.w3schools.com/tags/tag_details.asp"/>
-    <hyperlink ref="B30" r:id="rId29" display="https://www.w3schools.com/tags/tag_dfn.asp"/>
-    <hyperlink ref="B31" r:id="rId30" display="https://www.w3schools.com/tags/tag_dialog.asp"/>
-    <hyperlink ref="B32" r:id="rId31" display="https://www.w3schools.com/tags/tag_div.asp"/>
-    <hyperlink ref="B33" r:id="rId32" display="https://www.w3schools.com/tags/tag_dl.asp"/>
-    <hyperlink ref="B34" r:id="rId33" display="https://www.w3schools.com/tags/tag_dt.asp"/>
-    <hyperlink ref="B35" r:id="rId34" display="https://www.w3schools.com/tags/tag_em.asp"/>
-    <hyperlink ref="B36" r:id="rId35" display="https://www.w3schools.com/tags/tag_embed.asp"/>
-    <hyperlink ref="B37" r:id="rId36" display="https://www.w3schools.com/tags/tag_fieldset.asp"/>
-    <hyperlink ref="B38" r:id="rId37" display="https://www.w3schools.com/tags/tag_figcaption.asp"/>
-    <hyperlink ref="B39" r:id="rId38" display="https://www.w3schools.com/tags/tag_figure.asp"/>
-    <hyperlink ref="B40" r:id="rId39" display="https://www.w3schools.com/tags/tag_footer.asp"/>
-    <hyperlink ref="B41" r:id="rId40" display="https://www.w3schools.com/tags/tag_form.asp"/>
-    <hyperlink ref="B42" r:id="rId41" display="https://www.w3schools.com/tags/tag_hn.asp"/>
-    <hyperlink ref="B43" r:id="rId42" display="https://www.w3schools.com/tags/tag_head.asp"/>
-    <hyperlink ref="B44" r:id="rId43" display="https://www.w3schools.com/tags/tag_header.asp"/>
-    <hyperlink ref="B45" r:id="rId44" display="https://www.w3schools.com/tags/tag_hr.asp"/>
-    <hyperlink ref="B46" r:id="rId45" display="https://www.w3schools.com/tags/tag_html.asp"/>
-    <hyperlink ref="B47" r:id="rId46" display="https://www.w3schools.com/tags/tag_i.asp"/>
-    <hyperlink ref="B48" r:id="rId47" display="https://www.w3schools.com/tags/tag_iframe.asp"/>
-    <hyperlink ref="B49" r:id="rId48" display="https://www.w3schools.com/tags/tag_img.asp"/>
-    <hyperlink ref="B50" r:id="rId49" display="https://www.w3schools.com/tags/tag_input.asp"/>
-    <hyperlink ref="B51" r:id="rId50" display="https://www.w3schools.com/tags/tag_ins.asp"/>
-    <hyperlink ref="B52" r:id="rId51" display="https://www.w3schools.com/tags/tag_kbd.asp"/>
-    <hyperlink ref="B53" r:id="rId52" display="https://www.w3schools.com/tags/tag_label.asp"/>
-    <hyperlink ref="B54" r:id="rId53" display="https://www.w3schools.com/tags/tag_legend.asp"/>
-    <hyperlink ref="B55" r:id="rId54" display="https://www.w3schools.com/tags/tag_li.asp"/>
-    <hyperlink ref="B56" r:id="rId55" display="https://www.w3schools.com/tags/tag_link.asp"/>
-    <hyperlink ref="B57" r:id="rId56" display="https://www.w3schools.com/tags/tag_main.asp"/>
-    <hyperlink ref="B58" r:id="rId57" display="https://www.w3schools.com/tags/tag_map.asp"/>
-    <hyperlink ref="B59" r:id="rId58" display="https://www.w3schools.com/tags/tag_mark.asp"/>
-    <hyperlink ref="B60" r:id="rId59" display="https://www.w3schools.com/tags/tag_meta.asp"/>
-    <hyperlink ref="B61" r:id="rId60" display="https://www.w3schools.com/tags/tag_meter.asp"/>
-    <hyperlink ref="B62" r:id="rId61" display="https://www.w3schools.com/tags/tag_nav.asp"/>
-    <hyperlink ref="B63" r:id="rId62" display="https://www.w3schools.com/tags/tag_noscript.asp"/>
-    <hyperlink ref="B64" r:id="rId63" display="https://www.w3schools.com/tags/tag_object.asp"/>
-    <hyperlink ref="B65" r:id="rId64" display="https://www.w3schools.com/tags/tag_ol.asp"/>
-    <hyperlink ref="B66" r:id="rId65" display="https://www.w3schools.com/tags/tag_optgroup.asp"/>
-    <hyperlink ref="B67" r:id="rId66" display="https://www.w3schools.com/tags/tag_option.asp"/>
-    <hyperlink ref="B68" r:id="rId67" display="https://www.w3schools.com/tags/tag_output.asp"/>
-    <hyperlink ref="B69" r:id="rId68" display="https://www.w3schools.com/tags/tag_p.asp"/>
-    <hyperlink ref="B70" r:id="rId69" display="https://www.w3schools.com/tags/tag_param.asp"/>
-    <hyperlink ref="B71" r:id="rId70" display="https://www.w3schools.com/tags/tag_picture.asp"/>
-    <hyperlink ref="B72" r:id="rId71" display="https://www.w3schools.com/tags/tag_pre.asp"/>
-    <hyperlink ref="B73" r:id="rId72" display="https://www.w3schools.com/tags/tag_progress.asp"/>
-    <hyperlink ref="B74" r:id="rId73" display="https://www.w3schools.com/tags/tag_q.asp"/>
-    <hyperlink ref="B75" r:id="rId74" display="https://www.w3schools.com/tags/tag_rp.asp"/>
-    <hyperlink ref="B76" r:id="rId75" display="https://www.w3schools.com/tags/tag_rt.asp"/>
-    <hyperlink ref="B77" r:id="rId76" display="https://www.w3schools.com/tags/tag_ruby.asp"/>
-    <hyperlink ref="B78" r:id="rId77" display="https://www.w3schools.com/tags/tag_s.asp"/>
-    <hyperlink ref="B79" r:id="rId78" display="https://www.w3schools.com/tags/tag_samp.asp"/>
-    <hyperlink ref="B80" r:id="rId79" display="https://www.w3schools.com/tags/tag_script.asp"/>
-    <hyperlink ref="B81" r:id="rId80" display="https://www.w3schools.com/tags/tag_section.asp"/>
-    <hyperlink ref="B82" r:id="rId81" display="https://www.w3schools.com/tags/tag_select.asp"/>
-    <hyperlink ref="B83" r:id="rId82" display="https://www.w3schools.com/tags/tag_small.asp"/>
-    <hyperlink ref="B84" r:id="rId83" display="https://www.w3schools.com/tags/tag_source.asp"/>
-    <hyperlink ref="B85" r:id="rId84" display="https://www.w3schools.com/tags/tag_span.asp"/>
-    <hyperlink ref="B86" r:id="rId85" display="https://www.w3schools.com/tags/tag_strong.asp"/>
-    <hyperlink ref="B87" r:id="rId86" display="https://www.w3schools.com/tags/tag_style.asp"/>
-    <hyperlink ref="B88" r:id="rId87" display="https://www.w3schools.com/tags/tag_sub.asp"/>
-    <hyperlink ref="B89" r:id="rId88" display="https://www.w3schools.com/tags/tag_summary.asp"/>
-    <hyperlink ref="B90" r:id="rId89" display="https://www.w3schools.com/tags/tag_sup.asp"/>
-    <hyperlink ref="B91" r:id="rId90" display="https://www.w3schools.com/tags/tag_svg.asp"/>
-    <hyperlink ref="B92" r:id="rId91" display="https://www.w3schools.com/tags/tag_table.asp"/>
-    <hyperlink ref="B93" r:id="rId92" display="https://www.w3schools.com/tags/tag_tbody.asp"/>
-    <hyperlink ref="B94" r:id="rId93" display="https://www.w3schools.com/tags/tag_td.asp"/>
-    <hyperlink ref="B95" r:id="rId94" display="https://www.w3schools.com/tags/tag_template.asp"/>
-    <hyperlink ref="B96" r:id="rId95" display="https://www.w3schools.com/tags/tag_textarea.asp"/>
-    <hyperlink ref="B97" r:id="rId96" display="https://www.w3schools.com/tags/tag_tfoot.asp"/>
-    <hyperlink ref="B98" r:id="rId97" display="https://www.w3schools.com/tags/tag_th.asp"/>
-    <hyperlink ref="B99" r:id="rId98" display="https://www.w3schools.com/tags/tag_thead.asp"/>
-    <hyperlink ref="B100" r:id="rId99" display="https://www.w3schools.com/tags/tag_time.asp"/>
-    <hyperlink ref="B101" r:id="rId100" display="https://www.w3schools.com/tags/tag_title.asp"/>
-    <hyperlink ref="B102" r:id="rId101" display="https://www.w3schools.com/tags/tag_tr.asp"/>
-    <hyperlink ref="B103" r:id="rId102" display="https://www.w3schools.com/tags/tag_track.asp"/>
-    <hyperlink ref="B104" r:id="rId103" display="https://www.w3schools.com/tags/tag_u.asp"/>
-    <hyperlink ref="B105" r:id="rId104" display="https://www.w3schools.com/tags/tag_ul.asp"/>
-    <hyperlink ref="B106" r:id="rId105" display="https://www.w3schools.com/tags/tag_var.asp"/>
-    <hyperlink ref="B107" r:id="rId106" display="https://www.w3schools.com/tags/tag_video.asp"/>
-    <hyperlink ref="B108" r:id="rId107" display="https://www.w3schools.com/tags/tag_wbr.asp"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.w3schools.com/tags/tag_comment.asp" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.w3schools.com/tags/tag_doctype.asp" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.w3schools.com/tags/tag_a.asp" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.w3schools.com/tags/tag_abbr.asp" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.w3schools.com/tags/tag_address.asp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.w3schools.com/tags/tag_area.asp" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.w3schools.com/tags/tag_article.asp" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.w3schools.com/tags/tag_aside.asp" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.w3schools.com/tags/tag_audio.asp" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.w3schools.com/tags/tag_b.asp" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://www.w3schools.com/tags/tag_base.asp" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://www.w3schools.com/tags/tag_bdi.asp" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://www.w3schools.com/tags/tag_bdo.asp" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://www.w3schools.com/tags/tag_blockquote.asp" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://www.w3schools.com/tags/tag_body.asp" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://www.w3schools.com/tags/tag_br.asp" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://www.w3schools.com/tags/tag_button.asp" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://www.w3schools.com/tags/tag_canvas.asp" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" display="https://www.w3schools.com/tags/tag_caption.asp" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" display="https://www.w3schools.com/tags/tag_cite.asp" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://www.w3schools.com/tags/tag_code.asp" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://www.w3schools.com/tags/tag_col.asp" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://www.w3schools.com/tags/tag_colgroup.asp" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" display="https://www.w3schools.com/tags/tag_data.asp" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" display="https://www.w3schools.com/tags/tag_datalist.asp" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" display="https://www.w3schools.com/tags/tag_dd.asp" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" display="https://www.w3schools.com/tags/tag_del.asp" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" display="https://www.w3schools.com/tags/tag_details.asp" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" display="https://www.w3schools.com/tags/tag_dfn.asp" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" display="https://www.w3schools.com/tags/tag_dialog.asp" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" display="https://www.w3schools.com/tags/tag_div.asp" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" display="https://www.w3schools.com/tags/tag_dl.asp" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" display="https://www.w3schools.com/tags/tag_dt.asp" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" display="https://www.w3schools.com/tags/tag_em.asp" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" display="https://www.w3schools.com/tags/tag_embed.asp" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" display="https://www.w3schools.com/tags/tag_fieldset.asp" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" display="https://www.w3schools.com/tags/tag_figcaption.asp" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" display="https://www.w3schools.com/tags/tag_figure.asp" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" display="https://www.w3schools.com/tags/tag_footer.asp" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" display="https://www.w3schools.com/tags/tag_form.asp" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" display="https://www.w3schools.com/tags/tag_hn.asp" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" display="https://www.w3schools.com/tags/tag_head.asp" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" display="https://www.w3schools.com/tags/tag_header.asp" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" display="https://www.w3schools.com/tags/tag_hr.asp" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" display="https://www.w3schools.com/tags/tag_html.asp" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" display="https://www.w3schools.com/tags/tag_i.asp" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" display="https://www.w3schools.com/tags/tag_iframe.asp" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" display="https://www.w3schools.com/tags/tag_img.asp" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" display="https://www.w3schools.com/tags/tag_input.asp" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" display="https://www.w3schools.com/tags/tag_ins.asp" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" display="https://www.w3schools.com/tags/tag_kbd.asp" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" display="https://www.w3schools.com/tags/tag_label.asp" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" display="https://www.w3schools.com/tags/tag_legend.asp" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" display="https://www.w3schools.com/tags/tag_li.asp" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" display="https://www.w3schools.com/tags/tag_link.asp" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" display="https://www.w3schools.com/tags/tag_main.asp" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" display="https://www.w3schools.com/tags/tag_map.asp" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" display="https://www.w3schools.com/tags/tag_mark.asp" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" display="https://www.w3schools.com/tags/tag_meta.asp" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" display="https://www.w3schools.com/tags/tag_meter.asp" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" display="https://www.w3schools.com/tags/tag_nav.asp" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" display="https://www.w3schools.com/tags/tag_noscript.asp" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" display="https://www.w3schools.com/tags/tag_object.asp" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" display="https://www.w3schools.com/tags/tag_ol.asp" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" display="https://www.w3schools.com/tags/tag_optgroup.asp" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" display="https://www.w3schools.com/tags/tag_option.asp" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" display="https://www.w3schools.com/tags/tag_output.asp" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" display="https://www.w3schools.com/tags/tag_p.asp" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" display="https://www.w3schools.com/tags/tag_param.asp" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" display="https://www.w3schools.com/tags/tag_picture.asp" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" display="https://www.w3schools.com/tags/tag_pre.asp" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" display="https://www.w3schools.com/tags/tag_progress.asp" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" display="https://www.w3schools.com/tags/tag_q.asp" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" display="https://www.w3schools.com/tags/tag_rp.asp" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" display="https://www.w3schools.com/tags/tag_rt.asp" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" display="https://www.w3schools.com/tags/tag_ruby.asp" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" display="https://www.w3schools.com/tags/tag_s.asp" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" display="https://www.w3schools.com/tags/tag_samp.asp" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" display="https://www.w3schools.com/tags/tag_script.asp" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" display="https://www.w3schools.com/tags/tag_section.asp" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" display="https://www.w3schools.com/tags/tag_select.asp" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B83" r:id="rId82" display="https://www.w3schools.com/tags/tag_small.asp" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B84" r:id="rId83" display="https://www.w3schools.com/tags/tag_source.asp" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B85" r:id="rId84" display="https://www.w3schools.com/tags/tag_span.asp" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B86" r:id="rId85" display="https://www.w3schools.com/tags/tag_strong.asp" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B87" r:id="rId86" display="https://www.w3schools.com/tags/tag_style.asp" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B88" r:id="rId87" display="https://www.w3schools.com/tags/tag_sub.asp" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B89" r:id="rId88" display="https://www.w3schools.com/tags/tag_summary.asp" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B90" r:id="rId89" display="https://www.w3schools.com/tags/tag_sup.asp" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B91" r:id="rId90" display="https://www.w3schools.com/tags/tag_svg.asp" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B92" r:id="rId91" display="https://www.w3schools.com/tags/tag_table.asp" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B93" r:id="rId92" display="https://www.w3schools.com/tags/tag_tbody.asp" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B94" r:id="rId93" display="https://www.w3schools.com/tags/tag_td.asp" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B95" r:id="rId94" display="https://www.w3schools.com/tags/tag_template.asp" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B96" r:id="rId95" display="https://www.w3schools.com/tags/tag_textarea.asp" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B97" r:id="rId96" display="https://www.w3schools.com/tags/tag_tfoot.asp" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B98" r:id="rId97" display="https://www.w3schools.com/tags/tag_th.asp" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B99" r:id="rId98" display="https://www.w3schools.com/tags/tag_thead.asp" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B100" r:id="rId99" display="https://www.w3schools.com/tags/tag_time.asp" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B101" r:id="rId100" display="https://www.w3schools.com/tags/tag_title.asp" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B102" r:id="rId101" display="https://www.w3schools.com/tags/tag_tr.asp" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B103" r:id="rId102" display="https://www.w3schools.com/tags/tag_track.asp" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B104" r:id="rId103" display="https://www.w3schools.com/tags/tag_u.asp" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B105" r:id="rId104" display="https://www.w3schools.com/tags/tag_ul.asp" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B106" r:id="rId105" display="https://www.w3schools.com/tags/tag_var.asp" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B107" r:id="rId106" display="https://www.w3schools.com/tags/tag_video.asp" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B108" r:id="rId107" display="https://www.w3schools.com/tags/tag_wbr.asp" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>